<commit_message>
Add few String files
</commit_message>
<xml_diff>
--- a/FINAL450.xlsx
+++ b/FINAL450.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Love Babbar DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BACFC1-2662-45F9-8837-2A7426E3A9CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85067AEC-26D4-43F5-A456-726FDB448B31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="466">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1420,6 +1420,9 @@
   </si>
   <si>
     <t xml:space="preserve">Youtube Channel: https://www.youtube.com/channel/UCQHLxxBFrbfdrk1jF0moTpw </t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -1851,8 +1854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1896,7 +1899,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -2420,7 +2423,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="21">
@@ -2431,7 +2434,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21">
@@ -2464,7 +2467,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="21">

</xml_diff>